<commit_message>
redid some incorrect times on vectorization
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxdolan/Documents/Jupyter_lab_stuff/software engineering &amp; HPC/LebwohlLasher_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298CA8F7-FF7B-E847-856E-7FD0A55AD841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2131EBCD-274F-874F-AD1C-DC1ED601609A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="660" windowWidth="14180" windowHeight="14000" xr2:uid="{B7EF231A-720A-6B40-A29A-AACFB4BFB12D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{B7EF231A-720A-6B40-A29A-AACFB4BFB12D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D532BB28-C2FB-B24C-A4EF-BD09DCC39915}">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,7 +973,7 @@
         <v>21</v>
       </c>
       <c r="E15" s="2">
-        <v>3.2349999999999999</v>
+        <v>3.0430000000000001</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -985,7 +985,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="2">
-        <v>2.6120000000000001</v>
+        <v>2.4359999999999999</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -997,7 +997,7 @@
         <v>23</v>
       </c>
       <c r="E17" s="2">
-        <v>1.8</v>
+        <v>1.665</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -1009,7 +1009,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="2">
-        <v>1.6359999999999999</v>
+        <v>1.528</v>
       </c>
       <c r="F18" s="3"/>
       <c r="H18" t="s">
@@ -1024,7 +1024,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="2">
-        <v>1.823</v>
+        <v>3.1629999999999998</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -1036,7 +1036,7 @@
         <v>29</v>
       </c>
       <c r="E20" s="2">
-        <v>0.95699999999999996</v>
+        <v>1.5580000000000001</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -1155,11 +1155,11 @@
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>16</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="21" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="2">

</xml_diff>

<commit_message>
added new versions of numba scripts
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxdolan/Documents/Jupyter_lab_stuff/software engineering &amp; HPC/LebwohlLasher_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2131EBCD-274F-874F-AD1C-DC1ED601609A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A913F139-ABB7-0A40-A4DF-729780FFC0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{B7EF231A-720A-6B40-A29A-AACFB4BFB12D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t xml:space="preserve">method </t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>changed to be above one_energy and used nopython = True</t>
+  </si>
+  <si>
+    <t>set cache = true</t>
+  </si>
+  <si>
+    <t>cache = true</t>
   </si>
 </sst>
 </file>
@@ -791,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D532BB28-C2FB-B24C-A4EF-BD09DCC39915}">
-  <dimension ref="B1:H41"/>
+  <dimension ref="B1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,39 +1146,55 @@
       <c r="E28" s="2"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="29" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1.2170000000000001</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D30" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="2">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
+      <c r="E30" s="2">
+        <v>1.766</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D31" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E31" s="2">
         <v>0.67600000000000005</v>
       </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E31" s="2"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E32" s="2"/>
+    <row r="32" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.49199999999999999</v>
+      </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.2">
@@ -1210,6 +1232,10 @@
     <row r="41" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E41" s="2"/>
       <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E42" s="2"/>
+      <c r="F42" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>